<commit_message>
Calculation and export updates
</commit_message>
<xml_diff>
--- a/Test_File.xlsx
+++ b/Test_File.xlsx
@@ -17,7 +17,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="yyyy-mm-dd h:mm:ss"/>
+    <numFmt numFmtId="164" formatCode="yyyy-mm-dd"/>
   </numFmts>
   <fonts count="1">
     <font>
@@ -416,7 +416,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -462,6 +462,86 @@
         <v>0</v>
       </c>
     </row>
+    <row r="3">
+      <c r="A3" s="1" t="n">
+        <v>44631</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Paycheck</t>
+        </is>
+      </c>
+      <c r="C3" t="n">
+        <v>1350</v>
+      </c>
+      <c r="D3" t="n">
+        <v>1350</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="n">
+        <v>44640</v>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Pizza</t>
+        </is>
+      </c>
+      <c r="C4" t="n">
+        <v>-30</v>
+      </c>
+      <c r="D4" t="n">
+        <v>1320</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="n">
+        <v>44645</v>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Paycheck</t>
+        </is>
+      </c>
+      <c r="C5" t="n">
+        <v>1350</v>
+      </c>
+      <c r="D5" t="n">
+        <v>2670</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="1" t="n">
+        <v>44659</v>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Paycheck</t>
+        </is>
+      </c>
+      <c r="C6" t="n">
+        <v>1350</v>
+      </c>
+      <c r="D6" t="n">
+        <v>4020</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="1" t="n">
+        <v>44673</v>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>Paycheck</t>
+        </is>
+      </c>
+      <c r="C7" t="n">
+        <v>1350</v>
+      </c>
+      <c r="D7" t="n">
+        <v>5370</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>